<commit_message>
Tuples examples, Range.Replace,modified LED report template
</commit_message>
<xml_diff>
--- a/ConsoleApps/TemplateLED.xlsx
+++ b/ConsoleApps/TemplateLED.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Header" sheetId="1" r:id="rId1"/>
+    <sheet name="Report" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +19,20 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t xml:space="preserve">Titolo:   </t>
+  </si>
+  <si>
+    <t>&lt;TITLE&gt;</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +40,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +75,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -66,6 +99,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>540439</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>140844</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="769620" y="228600"/>
+          <a:ext cx="4647619" cy="1009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,12 +407,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:I10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="100" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>